<commit_message>
Layout dash fundamental done
</commit_message>
<xml_diff>
--- a/time spacing/words_test.xlsx
+++ b/time spacing/words_test.xlsx
@@ -437,10 +437,10 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>45213</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="2">
@@ -458,7 +458,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="3">
@@ -473,10 +473,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>45217</v>
+        <v>45227</v>
       </c>
     </row>
     <row r="4">
@@ -491,10 +491,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>45213</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="5">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>45213</v>
+        <v>45227</v>
       </c>
     </row>
     <row r="6">
@@ -530,7 +530,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="7">
@@ -548,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="8">
@@ -563,10 +563,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>45213</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="9">
@@ -581,10 +581,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>45213</v>
+        <v>45235</v>
       </c>
     </row>
     <row r="10">
@@ -599,10 +599,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>45213</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="11">
@@ -617,10 +617,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>45213</v>
+        <v>45227</v>
       </c>
     </row>
     <row r="12">
@@ -635,10 +635,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>45213</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="13">
@@ -653,10 +653,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>45213</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="14">
@@ -689,10 +689,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>45213</v>
+        <v>45225</v>
       </c>
     </row>
     <row r="16">
@@ -728,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>45213</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="18">
@@ -764,7 +764,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="20">
@@ -779,10 +779,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>45213</v>
+        <v>45227</v>
       </c>
     </row>
     <row r="21">
@@ -797,10 +797,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>45213</v>
+        <v>45233</v>
       </c>
     </row>
     <row r="22">
@@ -818,7 +818,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="23">
@@ -833,10 +833,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>45213</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="24">
@@ -851,10 +851,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>45213</v>
+        <v>45227</v>
       </c>
     </row>
     <row r="25">
@@ -869,10 +869,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>45217</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="26">
@@ -908,7 +908,7 @@
         <v>4</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>45217</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="28">
@@ -941,10 +941,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>45214</v>
+        <v>45223</v>
       </c>
     </row>
     <row r="30">
@@ -962,7 +962,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="31">
@@ -977,10 +977,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>45213</v>
+        <v>45233</v>
       </c>
     </row>
     <row r="32">
@@ -995,10 +995,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>45213</v>
+        <v>45233</v>
       </c>
     </row>
     <row r="33">
@@ -1016,7 +1016,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="34">
@@ -1031,10 +1031,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>45213</v>
+        <v>45225</v>
       </c>
     </row>
     <row r="35">
@@ -1049,10 +1049,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>45213</v>
+        <v>45227</v>
       </c>
     </row>
     <row r="36">
@@ -1070,7 +1070,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="37">
@@ -1103,10 +1103,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>45215</v>
+        <v>45222</v>
       </c>
     </row>
     <row r="39">
@@ -1121,10 +1121,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>45213</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="40">
@@ -1142,7 +1142,7 @@
         <v>2</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="41">
@@ -1157,10 +1157,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>45213</v>
+        <v>45225</v>
       </c>
     </row>
     <row r="42">
@@ -1175,10 +1175,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>45213</v>
+        <v>45222</v>
       </c>
     </row>
     <row r="43">
@@ -1193,10 +1193,10 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>45213</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="44">
@@ -1211,10 +1211,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>45213</v>
+        <v>45234</v>
       </c>
     </row>
     <row r="45">
@@ -1229,10 +1229,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>45213</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="46">
@@ -1247,10 +1247,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>45213</v>
+        <v>45235</v>
       </c>
     </row>
     <row r="47">
@@ -1283,10 +1283,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>45213</v>
+        <v>45222</v>
       </c>
     </row>
     <row r="49">
@@ -1304,7 +1304,7 @@
         <v>4</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>45217</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="50">
@@ -1319,10 +1319,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>45214</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="51">
@@ -1337,10 +1337,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>45213</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="52">
@@ -1355,10 +1355,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>45213</v>
+        <v>45222</v>
       </c>
     </row>
     <row r="53">
@@ -1391,10 +1391,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>45213</v>
+        <v>45225</v>
       </c>
     </row>
     <row r="55">
@@ -1412,7 +1412,7 @@
         <v>1</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>45213</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="56">
@@ -1427,10 +1427,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>45213</v>
+        <v>45222</v>
       </c>
     </row>
     <row r="57">
@@ -1445,10 +1445,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>45213</v>
+        <v>45234</v>
       </c>
     </row>
     <row r="58">
@@ -1463,10 +1463,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>45213</v>
+        <v>45234</v>
       </c>
     </row>
     <row r="59">
@@ -1484,7 +1484,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="60">
@@ -1520,7 +1520,7 @@
         <v>4</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="62">
@@ -1553,10 +1553,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>45213</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="64">
@@ -1571,10 +1571,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>45213</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="65">
@@ -1592,7 +1592,7 @@
         <v>8</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="66">
@@ -1607,10 +1607,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>45213</v>
+        <v>45222</v>
       </c>
     </row>
     <row r="67">
@@ -1643,10 +1643,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>45213</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="69">
@@ -1661,10 +1661,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>45213</v>
+        <v>45222</v>
       </c>
     </row>
     <row r="70">
@@ -1682,7 +1682,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>45214</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="71">
@@ -1697,10 +1697,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D71" s="1" t="n">
-        <v>45213</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="72">
@@ -1736,7 +1736,7 @@
         <v>4</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="74">
@@ -1751,10 +1751,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>45214</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="75">
@@ -1769,10 +1769,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D75" s="1" t="n">
-        <v>45213</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="76">
@@ -1790,7 +1790,7 @@
         <v>4</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>45214</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="77">
@@ -1805,10 +1805,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>45213</v>
+        <v>45227</v>
       </c>
     </row>
     <row r="78">
@@ -1823,10 +1823,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>45213</v>
+        <v>45223</v>
       </c>
     </row>
     <row r="79">
@@ -1841,10 +1841,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D79" s="1" t="n">
-        <v>45213</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="80">
@@ -1862,7 +1862,7 @@
         <v>8</v>
       </c>
       <c r="D80" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="81">
@@ -1877,10 +1877,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D81" s="1" t="n">
-        <v>45213</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="82">
@@ -1895,10 +1895,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D82" s="1" t="n">
-        <v>45213</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="83">
@@ -1916,7 +1916,7 @@
         <v>2</v>
       </c>
       <c r="D83" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="84">
@@ -1931,10 +1931,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>45213</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="85">
@@ -1952,7 +1952,7 @@
         <v>1</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="86">
@@ -1970,7 +1970,7 @@
         <v>2</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>45215</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="87">
@@ -2021,10 +2021,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>45214</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="90">
@@ -2039,10 +2039,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D90" s="1" t="n">
-        <v>45213</v>
+        <v>45227</v>
       </c>
     </row>
     <row r="91">
@@ -2057,10 +2057,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D91" s="1" t="n">
-        <v>45217</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="92">
@@ -2075,10 +2075,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D92" s="1" t="n">
-        <v>45213</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="93">
@@ -2093,10 +2093,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D93" s="1" t="n">
-        <v>45213</v>
+        <v>45227</v>
       </c>
     </row>
     <row r="94">
@@ -2111,10 +2111,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D94" s="1" t="n">
-        <v>45213</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="95">
@@ -2129,10 +2129,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D95" s="1" t="n">
-        <v>45213</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="96">
@@ -2150,7 +2150,7 @@
         <v>1</v>
       </c>
       <c r="D96" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="97">
@@ -2165,10 +2165,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>45214</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="98">
@@ -2183,10 +2183,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>45213</v>
+        <v>45223</v>
       </c>
     </row>
     <row r="99">
@@ -2204,7 +2204,7 @@
         <v>1</v>
       </c>
       <c r="D99" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="100">
@@ -2219,10 +2219,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>45213</v>
+        <v>45223</v>
       </c>
     </row>
     <row r="101">
@@ -2240,7 +2240,7 @@
         <v>1</v>
       </c>
       <c r="D101" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="102">
@@ -2255,10 +2255,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D102" s="1" t="n">
-        <v>45213</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="103">
@@ -2276,7 +2276,7 @@
         <v>2</v>
       </c>
       <c r="D103" s="1" t="n">
-        <v>45213</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="104">
@@ -2291,10 +2291,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D104" s="1" t="n">
-        <v>45215</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="105">
@@ -2312,7 +2312,7 @@
         <v>2</v>
       </c>
       <c r="D105" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="106">
@@ -2327,10 +2327,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D106" s="1" t="n">
-        <v>45214</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="107">
@@ -2345,10 +2345,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D107" s="1" t="n">
-        <v>45213</v>
+        <v>45234</v>
       </c>
     </row>
     <row r="108">
@@ -2366,7 +2366,7 @@
         <v>4</v>
       </c>
       <c r="D108" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="109">
@@ -2384,7 +2384,7 @@
         <v>1</v>
       </c>
       <c r="D109" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="110">
@@ -2399,10 +2399,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D110" s="1" t="n">
-        <v>45214</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="111">
@@ -2420,7 +2420,7 @@
         <v>1</v>
       </c>
       <c r="D111" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="112">
@@ -2435,10 +2435,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D112" s="1" t="n">
-        <v>45217</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="113">
@@ -2456,7 +2456,7 @@
         <v>1</v>
       </c>
       <c r="D113" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="114">
@@ -2489,10 +2489,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D115" s="1" t="n">
-        <v>45213</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="116">
@@ -2507,10 +2507,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D116" s="1" t="n">
-        <v>45213</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="117">
@@ -2525,10 +2525,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D117" s="1" t="n">
-        <v>45213</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="118">
@@ -2543,10 +2543,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D118" s="1" t="n">
-        <v>45213</v>
+        <v>45222</v>
       </c>
     </row>
     <row r="119">
@@ -2564,7 +2564,7 @@
         <v>4</v>
       </c>
       <c r="D119" s="1" t="n">
-        <v>45213</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="120">
@@ -2579,10 +2579,10 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D120" s="1" t="n">
-        <v>45213</v>
+        <v>45235</v>
       </c>
     </row>
     <row r="121">
@@ -2600,7 +2600,7 @@
         <v>2</v>
       </c>
       <c r="D121" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="122">
@@ -2615,10 +2615,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D122" s="1" t="n">
-        <v>45213</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="123">
@@ -2633,10 +2633,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D123" s="1" t="n">
-        <v>45213</v>
+        <v>45221</v>
       </c>
     </row>
     <row r="124">
@@ -2654,7 +2654,7 @@
         <v>1</v>
       </c>
       <c r="D124" s="1" t="n">
-        <v>45213</v>
+        <v>45219</v>
       </c>
     </row>
     <row r="125">
@@ -2669,10 +2669,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D125" s="1" t="n">
-        <v>45213</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="126">
@@ -2687,10 +2687,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D126" s="1" t="n">
-        <v>45213</v>
+        <v>45234</v>
       </c>
     </row>
     <row r="127">
@@ -2705,10 +2705,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D127" s="1" t="n">
-        <v>45213</v>
+        <v>45227</v>
       </c>
     </row>
     <row r="128">
@@ -2723,10 +2723,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D128" s="1" t="n">
-        <v>45213</v>
+        <v>45223</v>
       </c>
     </row>
     <row r="129">
@@ -2741,10 +2741,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D129" s="1" t="n">
-        <v>45213</v>
+        <v>45220</v>
       </c>
     </row>
     <row r="130">
@@ -2759,10 +2759,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D130" s="1" t="n">
-        <v>45213</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="131">
@@ -2777,10 +2777,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D131" s="1" t="n">
-        <v>45213</v>
+        <v>45220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>